<commit_message>
Fixed problem: was previously eliminating equal performance by same athlete if table for that record was updated later for another athlete
</commit_message>
<xml_diff>
--- a/CnC_known_historical.xlsx
+++ b/CnC_known_historical.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\powerof10-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C33027-6684-470C-9F39-A46C3E0FD1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE95FA52-0F3C-4BC7-8D8B-21185F944FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DE35B28A-4815-4142-AF1E-480F61EDA5DE}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -47,9 +47,6 @@
     <t>Use text format when pasting numbers!</t>
   </si>
   <si>
-    <t>But was this his PB for the club?</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://more.arrs.run/runner/15799 </t>
   </si>
   <si>
@@ -98,17 +95,23 @@
     <t>Fixture URL</t>
   </si>
   <si>
-    <t>Harlow (was this club PB?)</t>
-  </si>
-  <si>
     <t>Age Code</t>
+  </si>
+  <si>
+    <t>Harlow</t>
+  </si>
+  <si>
+    <t>This matches 2009 club records so must be right performance</t>
+  </si>
+  <si>
+    <t>Add known performances here (e.g. for road events) that predate powerof10 and are missing from the official C&amp;C T&amp;F records</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -142,6 +145,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -164,7 +174,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -181,6 +191,7 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -496,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6262A1C6-2E08-4627-9589-5880845FD58A}">
-  <dimension ref="A1:K58"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -510,85 +521,90 @@
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="7"/>
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="7"/>
+      <c r="B3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="6" t="s">
+      <c r="F3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="6" t="s">
+      <c r="K3" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>2</v>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
+    <row r="33" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A33" s="2"/>
     </row>
-    <row r="31" spans="1:1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
-    </row>
-    <row r="58" spans="1:1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
+    <row r="60" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{DA518F53-48F6-4384-B523-77D886998775}"/>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{DA518F53-48F6-4384-B523-77D886998775}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Graham Tuck 10M result added
</commit_message>
<xml_diff>
--- a/CnC_known_historical.xlsx
+++ b/CnC_known_historical.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\powerof10-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE95FA52-0F3C-4BC7-8D8B-21185F944FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DDB759-EA39-4D32-B5A7-4CDB28658FEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DE35B28A-4815-4142-AF1E-480F61EDA5DE}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -105,6 +105,21 @@
   </si>
   <si>
     <t>Add known performances here (e.g. for road events) that predate powerof10 and are missing from the official C&amp;C T&amp;F records</t>
+  </si>
+  <si>
+    <t>14 Oct ????</t>
+  </si>
+  <si>
+    <t>Mark Vile clipping ---&gt;</t>
+  </si>
+  <si>
+    <t>Walton</t>
+  </si>
+  <si>
+    <t>10M</t>
+  </si>
+  <si>
+    <t>47:12</t>
   </si>
 </sst>
 </file>
@@ -208,6 +223,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>241101</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>409574</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3418CAC5-04D5-AAE9-722B-32DC61547D57}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16519326" y="180974"/>
+          <a:ext cx="1387673" cy="3000375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -510,7 +580,7 @@
   <dimension ref="A1:K60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -589,9 +659,33 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="15" x14ac:dyDescent="0.2">
@@ -607,5 +701,6 @@
     <hyperlink ref="E4" r:id="rId1" xr:uid="{DA518F53-48F6-4384-B523-77D886998775}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Proper update with latest code; added Hannah Irwin's recent 10M as manual entry as not yet linked on po10
</commit_message>
<xml_diff>
--- a/CnC_known_historical.xlsx
+++ b/CnC_known_historical.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\powerof10-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DDB759-EA39-4D32-B5A7-4CDB28658FEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADEAEE61-BC98-48A3-AA31-28BADE20208D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DE35B28A-4815-4142-AF1E-480F61EDA5DE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DE35B28A-4815-4142-AF1E-480F61EDA5DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Other" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -120,6 +120,30 @@
   </si>
   <si>
     <t>47:12</t>
+  </si>
+  <si>
+    <t>54:30</t>
+  </si>
+  <si>
+    <t>15 Oct 2023</t>
+  </si>
+  <si>
+    <t>Hannah Irwin</t>
+  </si>
+  <si>
+    <t>Great South Run</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>https://www.runbritainrankings.com/results/results.aspx?meetingid=569139</t>
+  </si>
+  <si>
+    <t>https://www.thepowerof10.info/athletes/profile.aspx?athleteid=527586</t>
+  </si>
+  <si>
+    <t>Po10 not linking to Hannah's profile at 31Oct2023, submitted request</t>
   </si>
 </sst>
 </file>
@@ -579,24 +603,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6262A1C6-2E08-4627-9589-5880845FD58A}">
   <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="17.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="10" width="17.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="30.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="6" t="s">
         <v>14</v>
@@ -629,7 +653,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="5" t="s">
         <v>8</v>
@@ -659,7 +683,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -688,10 +712,42 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
     </row>
-    <row r="60" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>0</v>
       </c>
@@ -699,8 +755,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1" xr:uid="{DA518F53-48F6-4384-B523-77D886998775}"/>
+    <hyperlink ref="H6" r:id="rId2" xr:uid="{FEA18C4E-2D50-49F5-A2E8-08920EF4754E}"/>
+    <hyperlink ref="E6" r:id="rId3" xr:uid="{38A3E267-75A6-4A98-8478-B72ECBBB115E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Hannah Irwin's result on Po10 now
</commit_message>
<xml_diff>
--- a/CnC_known_historical.xlsx
+++ b/CnC_known_historical.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\powerof10-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADEAEE61-BC98-48A3-AA31-28BADE20208D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B876471E-CF8B-4FD0-9497-1760B6FCDDFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DE35B28A-4815-4142-AF1E-480F61EDA5DE}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -120,30 +120,6 @@
   </si>
   <si>
     <t>47:12</t>
-  </si>
-  <si>
-    <t>54:30</t>
-  </si>
-  <si>
-    <t>15 Oct 2023</t>
-  </si>
-  <si>
-    <t>Hannah Irwin</t>
-  </si>
-  <si>
-    <t>Great South Run</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>https://www.runbritainrankings.com/results/results.aspx?meetingid=569139</t>
-  </si>
-  <si>
-    <t>https://www.thepowerof10.info/athletes/profile.aspx?athleteid=527586</t>
-  </si>
-  <si>
-    <t>Po10 not linking to Hannah's profile at 31Oct2023, submitted request</t>
   </si>
 </sst>
 </file>
@@ -601,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6262A1C6-2E08-4627-9589-5880845FD58A}">
-  <dimension ref="A1:K60"/>
+  <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -712,53 +688,19 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>34</v>
-      </c>
+    <row r="32" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
     </row>
-    <row r="33" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-    </row>
-    <row r="60" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+    <row r="59" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1" xr:uid="{DA518F53-48F6-4384-B523-77D886998775}"/>
-    <hyperlink ref="H6" r:id="rId2" xr:uid="{FEA18C4E-2D50-49F5-A2E8-08920EF4754E}"/>
-    <hyperlink ref="E6" r:id="rId3" xr:uid="{38A3E267-75A6-4A98-8478-B72ECBBB115E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId4"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added logic to be able to invalidate records we know shouldn't be there (e.g. athlete still shown as club member on Po10/Runbritain but isn't actually), and created some entries for that. Changes order of some entries as files now processed last.
</commit_message>
<xml_diff>
--- a/CnC_known_historical.xlsx
+++ b/CnC_known_historical.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\powerof10-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B876471E-CF8B-4FD0-9497-1760B6FCDDFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAEF4A6-6848-4962-BEB3-55A6342FB436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DE35B28A-4815-4142-AF1E-480F61EDA5DE}"/>
+    <workbookView xWindow="2688" yWindow="948" windowWidth="17412" windowHeight="10704" xr2:uid="{DE35B28A-4815-4142-AF1E-480F61EDA5DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Other" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -120,6 +120,75 @@
   </si>
   <si>
     <t>47:12</t>
+  </si>
+  <si>
+    <t>7 Apr 2023</t>
+  </si>
+  <si>
+    <t>Paul Aste</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>"I wish I was still a member of C&amp;C but I think that expired in 2020"</t>
+  </si>
+  <si>
+    <t>30:45 INVALID</t>
+  </si>
+  <si>
+    <t>14:51 INVALID</t>
+  </si>
+  <si>
+    <t>11 May 2019</t>
+  </si>
+  <si>
+    <t>Ipswich</t>
+  </si>
+  <si>
+    <t>Port Erin</t>
+  </si>
+  <si>
+    <t>U23</t>
+  </si>
+  <si>
+    <t>5K</t>
+  </si>
+  <si>
+    <t>15:13.9 INVALID</t>
+  </si>
+  <si>
+    <t>3 Mar 2018</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>Lee Valley</t>
+  </si>
+  <si>
+    <t>Diane Potter</t>
+  </si>
+  <si>
+    <t>"I seem to have the club record for W60 5mile road race. Unfortunately, I'm no longer a member of C &amp; C and wasn't when I did the race"</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>V60</t>
+  </si>
+  <si>
+    <t>5M</t>
+  </si>
+  <si>
+    <t>26 Nov 2023</t>
+  </si>
+  <si>
+    <t>38:39 INVALID</t>
+  </si>
+  <si>
+    <t>Hatfield</t>
   </si>
 </sst>
 </file>
@@ -229,16 +298,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>241101</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>568761</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:rowOff>5714</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>409574</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>112394</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>106679</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -267,8 +336,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16519326" y="180974"/>
-          <a:ext cx="1387673" cy="3000375"/>
+          <a:off x="17965221" y="5714"/>
+          <a:ext cx="1418153" cy="3049905"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -580,7 +649,7 @@
   <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -688,6 +757,110 @@
         <v>23</v>
       </c>
     </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="32" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
     </row>

</xml_diff>

<commit_message>
Some historical hammer performances from Noel via Pete
</commit_message>
<xml_diff>
--- a/CnC_known_historical.xlsx
+++ b/CnC_known_historical.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\powerof10-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAEF4A6-6848-4962-BEB3-55A6342FB436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B860BCDD-D6EF-4FFA-81F0-D97D8C0A5576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="948" windowWidth="17412" windowHeight="10704" xr2:uid="{DE35B28A-4815-4142-AF1E-480F61EDA5DE}"/>
+    <workbookView xWindow="2304" yWindow="1404" windowWidth="17868" windowHeight="11556" xr2:uid="{DE35B28A-4815-4142-AF1E-480F61EDA5DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Other" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="64">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -189,6 +189,48 @@
   </si>
   <si>
     <t>Hatfield</t>
+  </si>
+  <si>
+    <t>19 Jun 1993</t>
+  </si>
+  <si>
+    <t>Perivale</t>
+  </si>
+  <si>
+    <t>From Noel Moss 8Apr2024</t>
+  </si>
+  <si>
+    <t>Nigel Spivey</t>
+  </si>
+  <si>
+    <t>56.42</t>
+  </si>
+  <si>
+    <t>HT7.26K</t>
+  </si>
+  <si>
+    <t>Simon Blackwell</t>
+  </si>
+  <si>
+    <t>Colchester</t>
+  </si>
+  <si>
+    <t>47.64</t>
+  </si>
+  <si>
+    <t>11 Sep 1994</t>
+  </si>
+  <si>
+    <t>Gary Parsons</t>
+  </si>
+  <si>
+    <t>1 Jul 1995</t>
+  </si>
+  <si>
+    <t>47.14</t>
+  </si>
+  <si>
+    <t>Welwyn</t>
   </si>
 </sst>
 </file>
@@ -648,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6262A1C6-2E08-4627-9589-5880845FD58A}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -861,6 +903,84 @@
         <v>43</v>
       </c>
     </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="32" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
     </row>

</xml_diff>

<commit_message>
PT's 5000m performance from 1996
</commit_message>
<xml_diff>
--- a/CnC_known_historical.xlsx
+++ b/CnC_known_historical.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\powerof10-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B860BCDD-D6EF-4FFA-81F0-D97D8C0A5576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9737B44E-0647-4599-8E5B-144B44B49CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="1404" windowWidth="17868" windowHeight="11556" xr2:uid="{DE35B28A-4815-4142-AF1E-480F61EDA5DE}"/>
+    <workbookView xWindow="1188" yWindow="480" windowWidth="17868" windowHeight="11556" xr2:uid="{DE35B28A-4815-4142-AF1E-480F61EDA5DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Other" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -231,6 +231,24 @@
   </si>
   <si>
     <t>Welwyn</t>
+  </si>
+  <si>
+    <t>15:30</t>
+  </si>
+  <si>
+    <t>3 Aug 1996</t>
+  </si>
+  <si>
+    <t>Pete Thompson</t>
+  </si>
+  <si>
+    <t>Portsmouth</t>
+  </si>
+  <si>
+    <t>V35</t>
+  </si>
+  <si>
+    <t>From Noel Moss 9Apr2024</t>
   </si>
 </sst>
 </file>
@@ -690,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6262A1C6-2E08-4627-9589-5880845FD58A}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -981,6 +999,32 @@
         <v>52</v>
       </c>
     </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
     <row r="32" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
     </row>

</xml_diff>

<commit_message>
Added Pete Thompson historical 5M & 10M results, but problem: only showing up as V35 not ALL currently.
</commit_message>
<xml_diff>
--- a/CnC_known_historical.xlsx
+++ b/CnC_known_historical.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\powerof10-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9737B44E-0647-4599-8E5B-144B44B49CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7AA345F-DBF9-49E9-93DB-0E6A04A7584A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1188" yWindow="480" windowWidth="17868" windowHeight="11556" xr2:uid="{DE35B28A-4815-4142-AF1E-480F61EDA5DE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DE35B28A-4815-4142-AF1E-480F61EDA5DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Other" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="78">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -249,6 +249,30 @@
   </si>
   <si>
     <t>From Noel Moss 9Apr2024</t>
+  </si>
+  <si>
+    <t>3 Jul 1997</t>
+  </si>
+  <si>
+    <t>25:59</t>
+  </si>
+  <si>
+    <t>Downham Market</t>
+  </si>
+  <si>
+    <t>See Ryston Runners screenshot --&gt;</t>
+  </si>
+  <si>
+    <t>1996</t>
+  </si>
+  <si>
+    <t>53:38</t>
+  </si>
+  <si>
+    <t>Bishops Stortford</t>
+  </si>
+  <si>
+    <t>See Stortford 10 screenshot --&gt;</t>
   </si>
 </sst>
 </file>
@@ -406,13 +430,101 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>287126</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>68579</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>371923</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>138590</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08D342BE-599B-1C39-DDED-D65DD7243705}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19558106" y="2011679"/>
+          <a:ext cx="3833837" cy="1243491"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>335280</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>10344</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>431203</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>62573</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C346DC6-6768-6820-6E64-BBC22F9D13C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17106900" y="2624004"/>
+          <a:ext cx="4469803" cy="1058069"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -450,7 +562,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -556,7 +668,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -698,7 +810,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -708,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6262A1C6-2E08-4627-9589-5880845FD58A}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1025,6 +1137,58 @@
         <v>69</v>
       </c>
     </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
     <row r="32" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
     </row>

</xml_diff>

<commit_message>
Peter not Pete Thompson for consistency
</commit_message>
<xml_diff>
--- a/CnC_known_historical.xlsx
+++ b/CnC_known_historical.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\powerof10-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7AA345F-DBF9-49E9-93DB-0E6A04A7584A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7892FEC-8CE3-4965-BE01-A4C78E6E55DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DE35B28A-4815-4142-AF1E-480F61EDA5DE}"/>
   </bookViews>
@@ -239,9 +239,6 @@
     <t>3 Aug 1996</t>
   </si>
   <si>
-    <t>Pete Thompson</t>
-  </si>
-  <si>
     <t>Portsmouth</t>
   </si>
   <si>
@@ -273,6 +270,9 @@
   </si>
   <si>
     <t>See Stortford 10 screenshot --&gt;</t>
+  </si>
+  <si>
+    <t>Peter Thompson</t>
   </si>
 </sst>
 </file>
@@ -821,7 +821,7 @@
   <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1119,74 +1119,74 @@
         <v>65</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>40</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ran C&C update, added Pete Thompson recent 10M performance not yet on po10
</commit_message>
<xml_diff>
--- a/CnC_known_historical.xlsx
+++ b/CnC_known_historical.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\powerof10-tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\powerof10-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7892FEC-8CE3-4965-BE01-A4C78E6E55DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95675061-3C65-4469-AFF0-D2C30F37D872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DE35B28A-4815-4142-AF1E-480F61EDA5DE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{DE35B28A-4815-4142-AF1E-480F61EDA5DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Other" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="84">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -273,6 +273,24 @@
   </si>
   <si>
     <t>Peter Thompson</t>
+  </si>
+  <si>
+    <t>V65</t>
+  </si>
+  <si>
+    <t>https://bmaf.opentrack.run/en-gb/x/2025/GBR/bmaf-10mile/event/1/1/1/</t>
+  </si>
+  <si>
+    <t>3 May 2025</t>
+  </si>
+  <si>
+    <t>69:37</t>
+  </si>
+  <si>
+    <t>Mallory Park</t>
+  </si>
+  <si>
+    <t>See URL or screenshot if that is now gone --&gt;</t>
   </si>
 </sst>
 </file>
@@ -432,16 +450,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>287126</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>68579</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>388726</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>36829</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>371923</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>138590</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>473523</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>81440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -464,8 +482,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="19558106" y="2011679"/>
-          <a:ext cx="3833837" cy="1243491"/>
+          <a:off x="21299276" y="792479"/>
+          <a:ext cx="3894797" cy="1181261"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -476,16 +494,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>335280</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>10344</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>557530</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>23044</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>431203</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>62573</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>18453</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>75273</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -508,8 +526,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17106900" y="2624004"/>
-          <a:ext cx="4469803" cy="1058069"/>
+          <a:off x="20833080" y="1915344"/>
+          <a:ext cx="4540923" cy="1004729"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>48119</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>203809</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>57275</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1591AB3C-53BF-169D-61B7-5BF6B79E87FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20491450" y="2892919"/>
+          <a:ext cx="6972909" cy="1437906"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -820,24 +882,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6262A1C6-2E08-4627-9589-5880845FD58A}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="17.33203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="30.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="1"/>
+    <col min="2" max="10" width="17.36328125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="30.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.08984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="6" t="s">
         <v>14</v>
@@ -870,7 +932,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="5" t="s">
         <v>8</v>
@@ -900,7 +962,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1189,10 +1251,39 @@
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
     </row>
-    <row r="59" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>0</v>
       </c>
@@ -1200,8 +1291,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1" xr:uid="{DA518F53-48F6-4384-B523-77D886998775}"/>
+    <hyperlink ref="H16" r:id="rId2" xr:uid="{5AFD5061-E0E2-4CD1-893D-97AB7D024121}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated, noted Ben Clarke's Valencia bib woes but on powerof10 anyway
</commit_message>
<xml_diff>
--- a/CnC_known_historical.xlsx
+++ b/CnC_known_historical.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\powerof10-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95675061-3C65-4469-AFF0-D2C30F37D872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4CF9A8-7B86-41A5-896F-0FD3BFAF7B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{DE35B28A-4815-4142-AF1E-480F61EDA5DE}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="91">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -291,6 +291,27 @@
   </si>
   <si>
     <t>See URL or screenshot if that is now gone --&gt;</t>
+  </si>
+  <si>
+    <t>Valencia</t>
+  </si>
+  <si>
+    <t>Screenshot - note Ben's bib disintegrated so didn't get a result initially, then organisers gave one though oddly 1.5 min quicker than own stopwatch result see https://www.strava.com/activities/16673378407</t>
+  </si>
+  <si>
+    <t>V55</t>
+  </si>
+  <si>
+    <t>2:43:00</t>
+  </si>
+  <si>
+    <t>7 Dec 2025</t>
+  </si>
+  <si>
+    <t>Ben Clarke</t>
+  </si>
+  <si>
+    <t>https://www.valenciaciudaddelrunning.com/en/marathon/2025-marathon-ranking/</t>
   </si>
 </sst>
 </file>
@@ -572,6 +593,50 @@
         <a:xfrm>
           <a:off x="20491450" y="2892919"/>
           <a:ext cx="6972909" cy="1437906"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>115752</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>134116</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>95685</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED91F475-9F2C-34BE-5797-9DE46CB4F30E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21026302" y="4895850"/>
+          <a:ext cx="11448364" cy="6509185"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -882,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6262A1C6-2E08-4627-9589-5880845FD58A}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1280,7 +1345,36 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
     </row>
     <row r="59" spans="1:1" ht="14.5" x14ac:dyDescent="0.25">
@@ -1292,8 +1386,9 @@
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1" xr:uid="{DA518F53-48F6-4384-B523-77D886998775}"/>
     <hyperlink ref="H16" r:id="rId2" xr:uid="{5AFD5061-E0E2-4CD1-893D-97AB7D024121}"/>
+    <hyperlink ref="H17" r:id="rId3" xr:uid="{8DC9337C-503C-44C4-BA48-F245BD1982AF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>